<commit_message>
CV pantall de notas de crédito, y formatos de exportación
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-NotCredito.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-NotCredito.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C328EF-271C-3D4C-AF5A-2B132720A3A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967C985B-E546-8A4C-BBE7-3560EEE6668E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="7840" windowWidth="56260" windowHeight="19800" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
+    <workbookView xWindow="9140" yWindow="12640" windowWidth="56260" windowHeight="19800" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
-  <si>
-    <t>% IVA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>ESTABLECIMEINTO :</t>
   </si>
@@ -42,18 +39,12 @@
     <t>HASTA:</t>
   </si>
   <si>
-    <t>N.</t>
-  </si>
-  <si>
     <t>FECHA EMISIÓN</t>
   </si>
   <si>
     <t>ESTADO</t>
   </si>
   <si>
-    <t>AUT S.R.I.</t>
-  </si>
-  <si>
     <t>SUBTOTAL</t>
   </si>
   <si>
@@ -72,24 +63,6 @@
     <t>DOC ASOCIADO</t>
   </si>
   <si>
-    <t>NOTAS DE CRÉDITO EMITIDAS</t>
-  </si>
-  <si>
-    <t>NOTA CRÉDITO</t>
-  </si>
-  <si>
-    <t>DETALLE</t>
-  </si>
-  <si>
-    <t>PRODUCTO / SERVICIO</t>
-  </si>
-  <si>
-    <t>CANTIDAD</t>
-  </si>
-  <si>
-    <t>P. UNITARIO</t>
-  </si>
-  <si>
     <t>DESC</t>
   </si>
   <si>
@@ -97,6 +70,12 @@
   </si>
   <si>
     <t>ICE</t>
+  </si>
+  <si>
+    <t>NOTAS DE CRÉDITO</t>
+  </si>
+  <si>
+    <t>NUM COMP</t>
   </si>
 </sst>
 </file>
@@ -142,7 +121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -170,51 +149,20 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -227,19 +175,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -556,202 +495,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32A76B9-2613-7147-BFF0-D21843D4C7F8}">
-  <dimension ref="A2:T10"/>
+  <dimension ref="A2:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
-    <col min="5" max="7" width="23.83203125" customWidth="1"/>
-    <col min="8" max="9" width="22.5" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5" customWidth="1"/>
-    <col min="12" max="12" width="13.5" customWidth="1"/>
-    <col min="13" max="13" width="37.83203125" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="11.5" customWidth="1"/>
-    <col min="20" max="20" width="13.5" customWidth="1"/>
+    <col min="1" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
+    <col min="6" max="8" width="23.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="8.5" customWidth="1"/>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="12"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="J9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="K9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="M9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="S10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="M9:T9"/>
+  <mergeCells count="5">
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>